<commit_message>
updated from 1980 to 2000
</commit_message>
<xml_diff>
--- a/theise from 1980 to 1990.xlsx
+++ b/theise from 1980 to 1990.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Coding\python\thesis-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D0E35F-129C-4BB6-A471-452CB1AAA6C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5366E7B3-C9AC-4C57-A6C8-D016A58C56CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7F6F008-BE90-4C20-9261-90C795ACE619}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="406">
   <si>
     <t>year</t>
   </si>
@@ -310,12 +310,6 @@
   </si>
   <si>
     <t>http://etheses.lse.ac.uk/1084/</t>
-  </si>
-  <si>
-    <t>Fendrich, Samuel</t>
-  </si>
-  <si>
-    <t>From axiomatization to generalizatrion of set theory.</t>
   </si>
   <si>
     <t>http://etheses.lse.ac.uk/3272/</t>
@@ -1263,6 +1257,21 @@
   </si>
   <si>
     <t>Tsai, Ing-Wen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fendrich, Samuel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://catalogue.libraries.london.ac.uk/search~S1/?searchtype=a&amp;searcharg=Fendrich%2C+Samuel&amp;searchscope=1&amp;sortdropdown=-&amp;SORT=D&amp;extended=0&amp;SUBMIT=Search&amp;searchlimits=&amp;searchorigarg=aBasanez%2C+Miguel</t>
+  </si>
+  <si>
+    <t>From axiomatization to generalizatrion of set theory.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generalizatrion should be generalization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1670,8 +1679,10 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1681,7 +1692,7 @@
     <col min="4" max="4" width="30.25" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="30.375" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1701,13 +1712,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2010,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1982</v>
       </c>
@@ -2030,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1982</v>
       </c>
@@ -2050,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1983</v>
       </c>
@@ -2070,12 +2081,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1983</v>
       </c>
       <c r="B20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
@@ -2090,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1984</v>
       </c>
@@ -2110,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1984</v>
       </c>
@@ -2130,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1984</v>
       </c>
@@ -2150,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1984</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1985</v>
       </c>
@@ -2190,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1985</v>
       </c>
@@ -2210,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1986</v>
       </c>
@@ -2230,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1986</v>
       </c>
@@ -2250,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1986</v>
       </c>
@@ -2270,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1987</v>
       </c>
@@ -2290,18 +2301,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1987</v>
       </c>
       <c r="B31" t="s">
+        <v>402</v>
+      </c>
+      <c r="C31" t="s">
+        <v>404</v>
+      </c>
+      <c r="D31" t="s">
         <v>91</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>93</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -2309,19 +2320,25 @@
       <c r="F31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>405</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1987</v>
       </c>
       <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
         <v>94</v>
-      </c>
-      <c r="C32" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" t="s">
-        <v>96</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -2335,13 +2352,13 @@
         <v>1987</v>
       </c>
       <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -2355,13 +2372,13 @@
         <v>1987</v>
       </c>
       <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" t="s">
         <v>100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" t="s">
-        <v>102</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -2375,13 +2392,13 @@
         <v>1988</v>
       </c>
       <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
         <v>103</v>
-      </c>
-      <c r="C35" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" t="s">
-        <v>105</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -2395,13 +2412,13 @@
         <v>1988</v>
       </c>
       <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
         <v>106</v>
-      </c>
-      <c r="C36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" t="s">
-        <v>108</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -2415,13 +2432,13 @@
         <v>1988</v>
       </c>
       <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
         <v>109</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" t="s">
-        <v>111</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
@@ -2435,13 +2452,13 @@
         <v>1989</v>
       </c>
       <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
         <v>112</v>
-      </c>
-      <c r="C38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>114</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -2455,13 +2472,13 @@
         <v>1989</v>
       </c>
       <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
         <v>115</v>
-      </c>
-      <c r="C39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" t="s">
-        <v>117</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -2475,13 +2492,13 @@
         <v>1989</v>
       </c>
       <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
         <v>118</v>
-      </c>
-      <c r="C40" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" t="s">
-        <v>120</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
@@ -2495,13 +2512,13 @@
         <v>1989</v>
       </c>
       <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" t="s">
         <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" t="s">
-        <v>123</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>
@@ -2515,13 +2532,13 @@
         <v>1989</v>
       </c>
       <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
         <v>124</v>
-      </c>
-      <c r="C42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" t="s">
-        <v>126</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
@@ -2535,13 +2552,13 @@
         <v>1989</v>
       </c>
       <c r="B43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
         <v>127</v>
-      </c>
-      <c r="C43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" t="s">
-        <v>129</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -2555,13 +2572,13 @@
         <v>1990</v>
       </c>
       <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
         <v>130</v>
-      </c>
-      <c r="C44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" t="s">
-        <v>132</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -2575,13 +2592,13 @@
         <v>1990</v>
       </c>
       <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" t="s">
         <v>133</v>
-      </c>
-      <c r="C45" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" t="s">
-        <v>135</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -2595,13 +2612,13 @@
         <v>1990</v>
       </c>
       <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" t="s">
         <v>136</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" t="s">
-        <v>138</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -2615,13 +2632,13 @@
         <v>1990</v>
       </c>
       <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" t="s">
         <v>139</v>
-      </c>
-      <c r="C47" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" t="s">
-        <v>141</v>
       </c>
       <c r="E47" t="b">
         <v>1</v>
@@ -2635,13 +2652,13 @@
         <v>1990</v>
       </c>
       <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" t="s">
         <v>142</v>
-      </c>
-      <c r="C48" t="s">
-        <v>143</v>
-      </c>
-      <c r="D48" t="s">
-        <v>144</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
@@ -2655,13 +2672,13 @@
         <v>1990</v>
       </c>
       <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" t="s">
         <v>145</v>
-      </c>
-      <c r="C49" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
@@ -2675,13 +2692,13 @@
         <v>1990</v>
       </c>
       <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
         <v>148</v>
-      </c>
-      <c r="C50" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" t="s">
-        <v>150</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -2695,13 +2712,13 @@
         <v>1990</v>
       </c>
       <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" t="s">
         <v>151</v>
-      </c>
-      <c r="C51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>153</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -2715,13 +2732,13 @@
         <v>1990</v>
       </c>
       <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
         <v>154</v>
-      </c>
-      <c r="C52" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52" t="s">
-        <v>156</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -2735,13 +2752,13 @@
         <v>1990</v>
       </c>
       <c r="B53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" t="s">
         <v>157</v>
-      </c>
-      <c r="C53" t="s">
-        <v>158</v>
-      </c>
-      <c r="D53" t="s">
-        <v>159</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -2755,13 +2772,13 @@
         <v>1990</v>
       </c>
       <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" t="s">
         <v>160</v>
-      </c>
-      <c r="C54" t="s">
-        <v>161</v>
-      </c>
-      <c r="D54" t="s">
-        <v>162</v>
       </c>
       <c r="E54" t="b">
         <v>1</v>
@@ -2775,13 +2792,13 @@
         <v>1990</v>
       </c>
       <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" t="s">
         <v>163</v>
-      </c>
-      <c r="C55" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" t="s">
-        <v>165</v>
       </c>
       <c r="E55" t="b">
         <v>1</v>
@@ -2795,13 +2812,13 @@
         <v>1990</v>
       </c>
       <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" t="s">
         <v>166</v>
-      </c>
-      <c r="C56" t="s">
-        <v>167</v>
-      </c>
-      <c r="D56" t="s">
-        <v>168</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
@@ -2815,13 +2832,13 @@
         <v>1990</v>
       </c>
       <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" t="s">
         <v>169</v>
-      </c>
-      <c r="C57" t="s">
-        <v>170</v>
-      </c>
-      <c r="D57" t="s">
-        <v>171</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
@@ -2835,13 +2852,13 @@
         <v>1990</v>
       </c>
       <c r="B58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" t="s">
         <v>172</v>
-      </c>
-      <c r="C58" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" t="s">
-        <v>174</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
@@ -2855,13 +2872,13 @@
         <v>1990</v>
       </c>
       <c r="B59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" t="s">
         <v>175</v>
-      </c>
-      <c r="C59" t="s">
-        <v>176</v>
-      </c>
-      <c r="D59" t="s">
-        <v>177</v>
       </c>
       <c r="E59" t="b">
         <v>1</v>
@@ -2875,13 +2892,13 @@
         <v>1990</v>
       </c>
       <c r="B60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" t="s">
         <v>178</v>
-      </c>
-      <c r="C60" t="s">
-        <v>179</v>
-      </c>
-      <c r="D60" t="s">
-        <v>180</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -2895,13 +2912,13 @@
         <v>1990</v>
       </c>
       <c r="B61" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" t="s">
         <v>181</v>
-      </c>
-      <c r="C61" t="s">
-        <v>182</v>
-      </c>
-      <c r="D61" t="s">
-        <v>183</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -2915,13 +2932,13 @@
         <v>1990</v>
       </c>
       <c r="B62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" t="s">
+        <v>183</v>
+      </c>
+      <c r="D62" t="s">
         <v>184</v>
-      </c>
-      <c r="C62" t="s">
-        <v>185</v>
-      </c>
-      <c r="D62" t="s">
-        <v>186</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -2935,13 +2952,13 @@
         <v>1990</v>
       </c>
       <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" t="s">
         <v>187</v>
-      </c>
-      <c r="C63" t="s">
-        <v>188</v>
-      </c>
-      <c r="D63" t="s">
-        <v>189</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -2955,13 +2972,13 @@
         <v>1990</v>
       </c>
       <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" t="s">
         <v>190</v>
-      </c>
-      <c r="C64" t="s">
-        <v>191</v>
-      </c>
-      <c r="D64" t="s">
-        <v>192</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -2975,13 +2992,13 @@
         <v>1990</v>
       </c>
       <c r="B65" t="s">
+        <v>191</v>
+      </c>
+      <c r="C65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" t="s">
         <v>193</v>
-      </c>
-      <c r="C65" t="s">
-        <v>194</v>
-      </c>
-      <c r="D65" t="s">
-        <v>195</v>
       </c>
       <c r="E65" t="b">
         <v>1</v>
@@ -2995,13 +3012,13 @@
         <v>1990</v>
       </c>
       <c r="B66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66" t="s">
         <v>196</v>
-      </c>
-      <c r="C66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D66" t="s">
-        <v>198</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
@@ -3015,13 +3032,13 @@
         <v>1990</v>
       </c>
       <c r="B67" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" t="s">
         <v>199</v>
-      </c>
-      <c r="C67" t="s">
-        <v>200</v>
-      </c>
-      <c r="D67" t="s">
-        <v>201</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
@@ -3035,13 +3052,13 @@
         <v>1990</v>
       </c>
       <c r="B68" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" t="s">
         <v>202</v>
-      </c>
-      <c r="C68" t="s">
-        <v>203</v>
-      </c>
-      <c r="D68" t="s">
-        <v>204</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
@@ -3055,13 +3072,13 @@
         <v>1990</v>
       </c>
       <c r="B69" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" t="s">
         <v>205</v>
-      </c>
-      <c r="C69" t="s">
-        <v>206</v>
-      </c>
-      <c r="D69" t="s">
-        <v>207</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
@@ -3075,13 +3092,13 @@
         <v>1990</v>
       </c>
       <c r="B70" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" t="s">
         <v>208</v>
-      </c>
-      <c r="C70" t="s">
-        <v>209</v>
-      </c>
-      <c r="D70" t="s">
-        <v>210</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
@@ -3095,13 +3112,13 @@
         <v>1990</v>
       </c>
       <c r="B71" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" t="s">
         <v>211</v>
-      </c>
-      <c r="C71" t="s">
-        <v>212</v>
-      </c>
-      <c r="D71" t="s">
-        <v>213</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -3115,13 +3132,13 @@
         <v>1990</v>
       </c>
       <c r="B72" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" t="s">
+        <v>213</v>
+      </c>
+      <c r="D72" t="s">
         <v>214</v>
-      </c>
-      <c r="C72" t="s">
-        <v>215</v>
-      </c>
-      <c r="D72" t="s">
-        <v>216</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
@@ -3135,13 +3152,13 @@
         <v>1990</v>
       </c>
       <c r="B73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" t="s">
         <v>217</v>
-      </c>
-      <c r="C73" t="s">
-        <v>218</v>
-      </c>
-      <c r="D73" t="s">
-        <v>219</v>
       </c>
       <c r="E73" t="b">
         <v>1</v>
@@ -3155,13 +3172,13 @@
         <v>1990</v>
       </c>
       <c r="B74" t="s">
+        <v>218</v>
+      </c>
+      <c r="C74" t="s">
+        <v>219</v>
+      </c>
+      <c r="D74" t="s">
         <v>220</v>
-      </c>
-      <c r="C74" t="s">
-        <v>221</v>
-      </c>
-      <c r="D74" t="s">
-        <v>222</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
@@ -3175,13 +3192,13 @@
         <v>1990</v>
       </c>
       <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" t="s">
+        <v>222</v>
+      </c>
+      <c r="D75" t="s">
         <v>223</v>
-      </c>
-      <c r="C75" t="s">
-        <v>224</v>
-      </c>
-      <c r="D75" t="s">
-        <v>225</v>
       </c>
       <c r="E75" t="b">
         <v>1</v>
@@ -3195,13 +3212,13 @@
         <v>1990</v>
       </c>
       <c r="B76" t="s">
+        <v>224</v>
+      </c>
+      <c r="C76" t="s">
+        <v>225</v>
+      </c>
+      <c r="D76" t="s">
         <v>226</v>
-      </c>
-      <c r="C76" t="s">
-        <v>227</v>
-      </c>
-      <c r="D76" t="s">
-        <v>228</v>
       </c>
       <c r="E76" t="b">
         <v>1</v>
@@ -3215,13 +3232,13 @@
         <v>1990</v>
       </c>
       <c r="B77" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" t="s">
+        <v>228</v>
+      </c>
+      <c r="D77" t="s">
         <v>229</v>
-      </c>
-      <c r="C77" t="s">
-        <v>230</v>
-      </c>
-      <c r="D77" t="s">
-        <v>231</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -3235,13 +3252,13 @@
         <v>1990</v>
       </c>
       <c r="B78" t="s">
+        <v>230</v>
+      </c>
+      <c r="C78" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" t="s">
         <v>232</v>
-      </c>
-      <c r="C78" t="s">
-        <v>233</v>
-      </c>
-      <c r="D78" t="s">
-        <v>234</v>
       </c>
       <c r="E78" t="b">
         <v>1</v>
@@ -3255,13 +3272,13 @@
         <v>1990</v>
       </c>
       <c r="B79" t="s">
+        <v>233</v>
+      </c>
+      <c r="C79" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" t="s">
         <v>235</v>
-      </c>
-      <c r="C79" t="s">
-        <v>236</v>
-      </c>
-      <c r="D79" t="s">
-        <v>237</v>
       </c>
       <c r="E79" t="b">
         <v>1</v>
@@ -3275,13 +3292,13 @@
         <v>1990</v>
       </c>
       <c r="B80" t="s">
+        <v>236</v>
+      </c>
+      <c r="C80" t="s">
+        <v>237</v>
+      </c>
+      <c r="D80" t="s">
         <v>238</v>
-      </c>
-      <c r="C80" t="s">
-        <v>239</v>
-      </c>
-      <c r="D80" t="s">
-        <v>240</v>
       </c>
       <c r="E80" t="b">
         <v>1</v>
@@ -3295,13 +3312,13 @@
         <v>1990</v>
       </c>
       <c r="B81" t="s">
+        <v>239</v>
+      </c>
+      <c r="C81" t="s">
+        <v>240</v>
+      </c>
+      <c r="D81" t="s">
         <v>241</v>
-      </c>
-      <c r="C81" t="s">
-        <v>242</v>
-      </c>
-      <c r="D81" t="s">
-        <v>243</v>
       </c>
       <c r="E81" t="b">
         <v>1</v>
@@ -3315,13 +3332,13 @@
         <v>1990</v>
       </c>
       <c r="B82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" t="s">
+        <v>243</v>
+      </c>
+      <c r="D82" t="s">
         <v>244</v>
-      </c>
-      <c r="C82" t="s">
-        <v>245</v>
-      </c>
-      <c r="D82" t="s">
-        <v>246</v>
       </c>
       <c r="E82" t="b">
         <v>1</v>
@@ -3335,13 +3352,13 @@
         <v>1990</v>
       </c>
       <c r="B83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" t="s">
+        <v>246</v>
+      </c>
+      <c r="D83" t="s">
         <v>247</v>
-      </c>
-      <c r="C83" t="s">
-        <v>248</v>
-      </c>
-      <c r="D83" t="s">
-        <v>249</v>
       </c>
       <c r="E83" t="b">
         <v>1</v>
@@ -3355,13 +3372,13 @@
         <v>1990</v>
       </c>
       <c r="B84" t="s">
+        <v>248</v>
+      </c>
+      <c r="C84" t="s">
+        <v>249</v>
+      </c>
+      <c r="D84" t="s">
         <v>250</v>
-      </c>
-      <c r="C84" t="s">
-        <v>251</v>
-      </c>
-      <c r="D84" t="s">
-        <v>252</v>
       </c>
       <c r="E84" t="b">
         <v>1</v>
@@ -3375,13 +3392,13 @@
         <v>1990</v>
       </c>
       <c r="B85" t="s">
+        <v>251</v>
+      </c>
+      <c r="C85" t="s">
+        <v>252</v>
+      </c>
+      <c r="D85" t="s">
         <v>253</v>
-      </c>
-      <c r="C85" t="s">
-        <v>254</v>
-      </c>
-      <c r="D85" t="s">
-        <v>255</v>
       </c>
       <c r="E85" t="b">
         <v>1</v>
@@ -3395,13 +3412,13 @@
         <v>1990</v>
       </c>
       <c r="B86" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" t="s">
+        <v>255</v>
+      </c>
+      <c r="D86" t="s">
         <v>256</v>
-      </c>
-      <c r="C86" t="s">
-        <v>257</v>
-      </c>
-      <c r="D86" t="s">
-        <v>258</v>
       </c>
       <c r="E86" t="b">
         <v>1</v>
@@ -3415,13 +3432,13 @@
         <v>1990</v>
       </c>
       <c r="B87" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D87" t="s">
         <v>259</v>
-      </c>
-      <c r="C87" t="s">
-        <v>260</v>
-      </c>
-      <c r="D87" t="s">
-        <v>261</v>
       </c>
       <c r="E87" t="b">
         <v>1</v>
@@ -3435,13 +3452,13 @@
         <v>1990</v>
       </c>
       <c r="B88" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" t="s">
         <v>262</v>
-      </c>
-      <c r="C88" t="s">
-        <v>263</v>
-      </c>
-      <c r="D88" t="s">
-        <v>264</v>
       </c>
       <c r="E88" t="b">
         <v>1</v>
@@ -3455,13 +3472,13 @@
         <v>1990</v>
       </c>
       <c r="B89" t="s">
+        <v>263</v>
+      </c>
+      <c r="C89" t="s">
+        <v>264</v>
+      </c>
+      <c r="D89" t="s">
         <v>265</v>
-      </c>
-      <c r="C89" t="s">
-        <v>266</v>
-      </c>
-      <c r="D89" t="s">
-        <v>267</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
@@ -3475,13 +3492,13 @@
         <v>1990</v>
       </c>
       <c r="B90" t="s">
+        <v>266</v>
+      </c>
+      <c r="C90" t="s">
+        <v>267</v>
+      </c>
+      <c r="D90" t="s">
         <v>268</v>
-      </c>
-      <c r="C90" t="s">
-        <v>269</v>
-      </c>
-      <c r="D90" t="s">
-        <v>270</v>
       </c>
       <c r="E90" t="b">
         <v>1</v>
@@ -3495,13 +3512,13 @@
         <v>1990</v>
       </c>
       <c r="B91" t="s">
+        <v>269</v>
+      </c>
+      <c r="C91" t="s">
+        <v>270</v>
+      </c>
+      <c r="D91" t="s">
         <v>271</v>
-      </c>
-      <c r="C91" t="s">
-        <v>272</v>
-      </c>
-      <c r="D91" t="s">
-        <v>273</v>
       </c>
       <c r="E91" t="b">
         <v>1</v>
@@ -3515,13 +3532,13 @@
         <v>1990</v>
       </c>
       <c r="B92" t="s">
+        <v>272</v>
+      </c>
+      <c r="C92" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" t="s">
         <v>274</v>
-      </c>
-      <c r="C92" t="s">
-        <v>275</v>
-      </c>
-      <c r="D92" t="s">
-        <v>276</v>
       </c>
       <c r="E92" t="b">
         <v>1</v>
@@ -3535,13 +3552,13 @@
         <v>1990</v>
       </c>
       <c r="B93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" t="s">
         <v>277</v>
-      </c>
-      <c r="C93" t="s">
-        <v>278</v>
-      </c>
-      <c r="D93" t="s">
-        <v>279</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -3555,13 +3572,13 @@
         <v>1990</v>
       </c>
       <c r="B94" t="s">
+        <v>278</v>
+      </c>
+      <c r="C94" t="s">
+        <v>279</v>
+      </c>
+      <c r="D94" t="s">
         <v>280</v>
-      </c>
-      <c r="C94" t="s">
-        <v>281</v>
-      </c>
-      <c r="D94" t="s">
-        <v>282</v>
       </c>
       <c r="E94" t="b">
         <v>1</v>
@@ -3575,13 +3592,13 @@
         <v>1990</v>
       </c>
       <c r="B95" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C95" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D95" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -3590,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="G95" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3601,13 +3618,13 @@
         <v>1990</v>
       </c>
       <c r="B96" t="s">
+        <v>282</v>
+      </c>
+      <c r="C96" t="s">
+        <v>283</v>
+      </c>
+      <c r="D96" t="s">
         <v>284</v>
-      </c>
-      <c r="C96" t="s">
-        <v>285</v>
-      </c>
-      <c r="D96" t="s">
-        <v>286</v>
       </c>
       <c r="E96" t="b">
         <v>1</v>
@@ -3621,13 +3638,13 @@
         <v>1990</v>
       </c>
       <c r="B97" t="s">
+        <v>285</v>
+      </c>
+      <c r="C97" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" t="s">
         <v>287</v>
-      </c>
-      <c r="C97" t="s">
-        <v>288</v>
-      </c>
-      <c r="D97" t="s">
-        <v>289</v>
       </c>
       <c r="E97" t="b">
         <v>1</v>
@@ -3641,13 +3658,13 @@
         <v>1990</v>
       </c>
       <c r="B98" t="s">
+        <v>288</v>
+      </c>
+      <c r="C98" t="s">
+        <v>289</v>
+      </c>
+      <c r="D98" t="s">
         <v>290</v>
-      </c>
-      <c r="C98" t="s">
-        <v>291</v>
-      </c>
-      <c r="D98" t="s">
-        <v>292</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
@@ -3661,13 +3678,13 @@
         <v>1990</v>
       </c>
       <c r="B99" t="s">
+        <v>291</v>
+      </c>
+      <c r="C99" t="s">
+        <v>292</v>
+      </c>
+      <c r="D99" t="s">
         <v>293</v>
-      </c>
-      <c r="C99" t="s">
-        <v>294</v>
-      </c>
-      <c r="D99" t="s">
-        <v>295</v>
       </c>
       <c r="E99" t="b">
         <v>1</v>
@@ -3681,13 +3698,13 @@
         <v>1990</v>
       </c>
       <c r="B100" t="s">
+        <v>294</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
+      <c r="D100" t="s">
         <v>296</v>
-      </c>
-      <c r="C100" t="s">
-        <v>297</v>
-      </c>
-      <c r="D100" t="s">
-        <v>298</v>
       </c>
       <c r="E100" t="b">
         <v>1</v>
@@ -3701,13 +3718,13 @@
         <v>1990</v>
       </c>
       <c r="B101" t="s">
+        <v>297</v>
+      </c>
+      <c r="C101" t="s">
+        <v>298</v>
+      </c>
+      <c r="D101" t="s">
         <v>299</v>
-      </c>
-      <c r="C101" t="s">
-        <v>300</v>
-      </c>
-      <c r="D101" t="s">
-        <v>301</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -3721,13 +3738,13 @@
         <v>1990</v>
       </c>
       <c r="B102" t="s">
+        <v>300</v>
+      </c>
+      <c r="C102" t="s">
+        <v>301</v>
+      </c>
+      <c r="D102" t="s">
         <v>302</v>
-      </c>
-      <c r="C102" t="s">
-        <v>303</v>
-      </c>
-      <c r="D102" t="s">
-        <v>304</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
@@ -3741,13 +3758,13 @@
         <v>1990</v>
       </c>
       <c r="B103" t="s">
+        <v>303</v>
+      </c>
+      <c r="C103" t="s">
+        <v>304</v>
+      </c>
+      <c r="D103" t="s">
         <v>305</v>
-      </c>
-      <c r="C103" t="s">
-        <v>306</v>
-      </c>
-      <c r="D103" t="s">
-        <v>307</v>
       </c>
       <c r="E103" t="b">
         <v>1</v>
@@ -3761,13 +3778,13 @@
         <v>1990</v>
       </c>
       <c r="B104" t="s">
+        <v>306</v>
+      </c>
+      <c r="C104" t="s">
+        <v>307</v>
+      </c>
+      <c r="D104" t="s">
         <v>308</v>
-      </c>
-      <c r="C104" t="s">
-        <v>309</v>
-      </c>
-      <c r="D104" t="s">
-        <v>310</v>
       </c>
       <c r="E104" t="b">
         <v>1</v>
@@ -3781,13 +3798,13 @@
         <v>1990</v>
       </c>
       <c r="B105" t="s">
+        <v>309</v>
+      </c>
+      <c r="C105" t="s">
+        <v>310</v>
+      </c>
+      <c r="D105" t="s">
         <v>311</v>
-      </c>
-      <c r="C105" t="s">
-        <v>312</v>
-      </c>
-      <c r="D105" t="s">
-        <v>313</v>
       </c>
       <c r="E105" t="b">
         <v>1</v>
@@ -3801,13 +3818,13 @@
         <v>1990</v>
       </c>
       <c r="B106" t="s">
+        <v>312</v>
+      </c>
+      <c r="C106" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" t="s">
         <v>314</v>
-      </c>
-      <c r="C106" t="s">
-        <v>315</v>
-      </c>
-      <c r="D106" t="s">
-        <v>316</v>
       </c>
       <c r="E106" t="b">
         <v>1</v>
@@ -3821,13 +3838,13 @@
         <v>1990</v>
       </c>
       <c r="B107" t="s">
+        <v>315</v>
+      </c>
+      <c r="C107" t="s">
+        <v>316</v>
+      </c>
+      <c r="D107" t="s">
         <v>317</v>
-      </c>
-      <c r="C107" t="s">
-        <v>318</v>
-      </c>
-      <c r="D107" t="s">
-        <v>319</v>
       </c>
       <c r="E107" t="b">
         <v>1</v>
@@ -3841,13 +3858,13 @@
         <v>1990</v>
       </c>
       <c r="B108" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C108" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D108" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E108" t="b">
         <v>0</v>
@@ -3856,10 +3873,10 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H108" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3867,13 +3884,13 @@
         <v>1990</v>
       </c>
       <c r="B109" t="s">
+        <v>319</v>
+      </c>
+      <c r="C109" t="s">
+        <v>320</v>
+      </c>
+      <c r="D109" t="s">
         <v>321</v>
-      </c>
-      <c r="C109" t="s">
-        <v>322</v>
-      </c>
-      <c r="D109" t="s">
-        <v>323</v>
       </c>
       <c r="E109" t="b">
         <v>1</v>
@@ -3887,13 +3904,13 @@
         <v>1990</v>
       </c>
       <c r="B110" t="s">
+        <v>322</v>
+      </c>
+      <c r="C110" t="s">
+        <v>323</v>
+      </c>
+      <c r="D110" t="s">
         <v>324</v>
-      </c>
-      <c r="C110" t="s">
-        <v>325</v>
-      </c>
-      <c r="D110" t="s">
-        <v>326</v>
       </c>
       <c r="E110" t="b">
         <v>1</v>
@@ -3907,13 +3924,13 @@
         <v>1990</v>
       </c>
       <c r="B111" t="s">
+        <v>325</v>
+      </c>
+      <c r="C111" t="s">
+        <v>326</v>
+      </c>
+      <c r="D111" t="s">
         <v>327</v>
-      </c>
-      <c r="C111" t="s">
-        <v>328</v>
-      </c>
-      <c r="D111" t="s">
-        <v>329</v>
       </c>
       <c r="E111" t="b">
         <v>1</v>
@@ -3927,13 +3944,13 @@
         <v>1990</v>
       </c>
       <c r="B112" t="s">
+        <v>328</v>
+      </c>
+      <c r="C112" t="s">
+        <v>329</v>
+      </c>
+      <c r="D112" t="s">
         <v>330</v>
-      </c>
-      <c r="C112" t="s">
-        <v>331</v>
-      </c>
-      <c r="D112" t="s">
-        <v>332</v>
       </c>
       <c r="E112" t="b">
         <v>1</v>
@@ -3947,13 +3964,13 @@
         <v>1990</v>
       </c>
       <c r="B113" t="s">
+        <v>331</v>
+      </c>
+      <c r="C113" t="s">
+        <v>332</v>
+      </c>
+      <c r="D113" t="s">
         <v>333</v>
-      </c>
-      <c r="C113" t="s">
-        <v>334</v>
-      </c>
-      <c r="D113" t="s">
-        <v>335</v>
       </c>
       <c r="E113" t="b">
         <v>1</v>
@@ -3967,13 +3984,13 @@
         <v>1990</v>
       </c>
       <c r="B114" t="s">
+        <v>334</v>
+      </c>
+      <c r="C114" t="s">
+        <v>335</v>
+      </c>
+      <c r="D114" t="s">
         <v>336</v>
-      </c>
-      <c r="C114" t="s">
-        <v>337</v>
-      </c>
-      <c r="D114" t="s">
-        <v>338</v>
       </c>
       <c r="E114" t="b">
         <v>1</v>
@@ -3987,13 +4004,13 @@
         <v>1990</v>
       </c>
       <c r="B115" t="s">
+        <v>337</v>
+      </c>
+      <c r="C115" t="s">
+        <v>338</v>
+      </c>
+      <c r="D115" t="s">
         <v>339</v>
-      </c>
-      <c r="C115" t="s">
-        <v>340</v>
-      </c>
-      <c r="D115" t="s">
-        <v>341</v>
       </c>
       <c r="E115" t="b">
         <v>1</v>
@@ -4007,13 +4024,13 @@
         <v>1990</v>
       </c>
       <c r="B116" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C116" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D116" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -4022,10 +4039,10 @@
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4033,13 +4050,13 @@
         <v>1990</v>
       </c>
       <c r="B117" t="s">
+        <v>341</v>
+      </c>
+      <c r="C117" t="s">
+        <v>342</v>
+      </c>
+      <c r="D117" t="s">
         <v>343</v>
-      </c>
-      <c r="C117" t="s">
-        <v>344</v>
-      </c>
-      <c r="D117" t="s">
-        <v>345</v>
       </c>
       <c r="E117" t="b">
         <v>1</v>
@@ -4053,13 +4070,13 @@
         <v>1990</v>
       </c>
       <c r="B118" t="s">
+        <v>344</v>
+      </c>
+      <c r="C118" t="s">
+        <v>345</v>
+      </c>
+      <c r="D118" t="s">
         <v>346</v>
-      </c>
-      <c r="C118" t="s">
-        <v>347</v>
-      </c>
-      <c r="D118" t="s">
-        <v>348</v>
       </c>
       <c r="E118" t="b">
         <v>1</v>
@@ -4073,13 +4090,13 @@
         <v>1990</v>
       </c>
       <c r="B119" t="s">
+        <v>347</v>
+      </c>
+      <c r="C119" t="s">
+        <v>348</v>
+      </c>
+      <c r="D119" t="s">
         <v>349</v>
-      </c>
-      <c r="C119" t="s">
-        <v>350</v>
-      </c>
-      <c r="D119" t="s">
-        <v>351</v>
       </c>
       <c r="E119" t="b">
         <v>1</v>
@@ -4093,13 +4110,13 @@
         <v>1990</v>
       </c>
       <c r="B120" t="s">
+        <v>350</v>
+      </c>
+      <c r="C120" t="s">
+        <v>351</v>
+      </c>
+      <c r="D120" t="s">
         <v>352</v>
-      </c>
-      <c r="C120" t="s">
-        <v>353</v>
-      </c>
-      <c r="D120" t="s">
-        <v>354</v>
       </c>
       <c r="E120" t="b">
         <v>1</v>
@@ -4113,13 +4130,13 @@
         <v>1990</v>
       </c>
       <c r="B121" t="s">
+        <v>353</v>
+      </c>
+      <c r="C121" t="s">
+        <v>354</v>
+      </c>
+      <c r="D121" t="s">
         <v>355</v>
-      </c>
-      <c r="C121" t="s">
-        <v>356</v>
-      </c>
-      <c r="D121" t="s">
-        <v>357</v>
       </c>
       <c r="E121" t="b">
         <v>1</v>
@@ -4133,13 +4150,13 @@
         <v>1990</v>
       </c>
       <c r="B122" t="s">
+        <v>356</v>
+      </c>
+      <c r="C122" t="s">
+        <v>357</v>
+      </c>
+      <c r="D122" t="s">
         <v>358</v>
-      </c>
-      <c r="C122" t="s">
-        <v>359</v>
-      </c>
-      <c r="D122" t="s">
-        <v>360</v>
       </c>
       <c r="E122" t="b">
         <v>1</v>
@@ -4153,13 +4170,13 @@
         <v>1990</v>
       </c>
       <c r="B123" t="s">
+        <v>359</v>
+      </c>
+      <c r="C123" t="s">
+        <v>360</v>
+      </c>
+      <c r="D123" t="s">
         <v>361</v>
-      </c>
-      <c r="C123" t="s">
-        <v>362</v>
-      </c>
-      <c r="D123" t="s">
-        <v>363</v>
       </c>
       <c r="E123" t="b">
         <v>1</v>
@@ -4173,13 +4190,13 @@
         <v>1990</v>
       </c>
       <c r="B124" t="s">
+        <v>362</v>
+      </c>
+      <c r="C124" t="s">
+        <v>363</v>
+      </c>
+      <c r="D124" t="s">
         <v>364</v>
-      </c>
-      <c r="C124" t="s">
-        <v>365</v>
-      </c>
-      <c r="D124" t="s">
-        <v>366</v>
       </c>
       <c r="E124" t="b">
         <v>1</v>
@@ -4193,13 +4210,13 @@
         <v>1990</v>
       </c>
       <c r="B125" t="s">
+        <v>365</v>
+      </c>
+      <c r="C125" t="s">
+        <v>366</v>
+      </c>
+      <c r="D125" t="s">
         <v>367</v>
-      </c>
-      <c r="C125" t="s">
-        <v>368</v>
-      </c>
-      <c r="D125" t="s">
-        <v>369</v>
       </c>
       <c r="E125" t="b">
         <v>1</v>
@@ -4213,13 +4230,13 @@
         <v>1990</v>
       </c>
       <c r="B126" t="s">
+        <v>368</v>
+      </c>
+      <c r="C126" t="s">
+        <v>369</v>
+      </c>
+      <c r="D126" t="s">
         <v>370</v>
-      </c>
-      <c r="C126" t="s">
-        <v>371</v>
-      </c>
-      <c r="D126" t="s">
-        <v>372</v>
       </c>
       <c r="E126" t="b">
         <v>1</v>
@@ -4233,13 +4250,13 @@
         <v>1990</v>
       </c>
       <c r="B127" t="s">
+        <v>371</v>
+      </c>
+      <c r="C127" t="s">
+        <v>372</v>
+      </c>
+      <c r="D127" t="s">
         <v>373</v>
-      </c>
-      <c r="C127" t="s">
-        <v>374</v>
-      </c>
-      <c r="D127" t="s">
-        <v>375</v>
       </c>
       <c r="E127" t="b">
         <v>1</v>
@@ -4253,13 +4270,13 @@
         <v>1990</v>
       </c>
       <c r="B128" t="s">
+        <v>374</v>
+      </c>
+      <c r="C128" t="s">
+        <v>375</v>
+      </c>
+      <c r="D128" t="s">
         <v>376</v>
-      </c>
-      <c r="C128" t="s">
-        <v>377</v>
-      </c>
-      <c r="D128" t="s">
-        <v>378</v>
       </c>
       <c r="E128" t="b">
         <v>1</v>
@@ -4273,13 +4290,13 @@
         <v>1990</v>
       </c>
       <c r="B129" t="s">
+        <v>377</v>
+      </c>
+      <c r="C129" t="s">
+        <v>378</v>
+      </c>
+      <c r="D129" t="s">
         <v>379</v>
-      </c>
-      <c r="C129" t="s">
-        <v>380</v>
-      </c>
-      <c r="D129" t="s">
-        <v>381</v>
       </c>
       <c r="E129" t="b">
         <v>1</v>
@@ -4293,13 +4310,13 @@
         <v>1990</v>
       </c>
       <c r="B130" t="s">
+        <v>380</v>
+      </c>
+      <c r="C130" t="s">
+        <v>381</v>
+      </c>
+      <c r="D130" t="s">
         <v>382</v>
-      </c>
-      <c r="C130" t="s">
-        <v>383</v>
-      </c>
-      <c r="D130" t="s">
-        <v>384</v>
       </c>
       <c r="E130" t="b">
         <v>1</v>
@@ -4313,13 +4330,13 @@
         <v>1990</v>
       </c>
       <c r="B131" t="s">
+        <v>383</v>
+      </c>
+      <c r="C131" t="s">
+        <v>384</v>
+      </c>
+      <c r="D131" t="s">
         <v>385</v>
-      </c>
-      <c r="C131" t="s">
-        <v>386</v>
-      </c>
-      <c r="D131" t="s">
-        <v>387</v>
       </c>
       <c r="E131" t="b">
         <v>1</v>
@@ -4335,7 +4352,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G108 G1:H1 G95 F1:F131 G116:H116">
+  <conditionalFormatting sqref="G108 G1:H1 G95 F1:F131 G116:H116 G31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -4343,8 +4360,9 @@
   <hyperlinks>
     <hyperlink ref="H95" r:id="rId1" xr:uid="{6B7405DF-6EA9-4D39-89A0-DF6A8046CD8C}"/>
     <hyperlink ref="H116" r:id="rId2" xr:uid="{10321EEE-8289-45BB-BF89-A3CB5710D272}"/>
+    <hyperlink ref="H31" r:id="rId3" xr:uid="{6656E936-ED26-4562-A7B6-B3F8910162C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>